<commit_message>
Change Pickle for Dill, minor changes
</commit_message>
<xml_diff>
--- a/tests/fixtures/excel_example_output.xlsx
+++ b/tests/fixtures/excel_example_output.xlsx
@@ -15,67 +15,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tmp2
-</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B                                                 </t>
-  </si>
-  <si>
-    <t>99.1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+  <si>
+    <t>jmeno</t>
+  </si>
+  <si>
+    <t>prijimeni</t>
+  </si>
+  <si>
+    <t>vek</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Novák</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>tmp1</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P                                                 </t>
-  </si>
-  <si>
-    <t>1.2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>tmp3</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O                                                 </t>
-  </si>
-  <si>
-    <t>0.2</t>
+    <t>Petr</t>
+  </si>
+  <si>
+    <t>Novotný</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Ondra</t>
+  </si>
+  <si>
+    <t>Pleticha</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Zuzana</t>
+  </si>
+  <si>
+    <t>Hánová</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -411,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -419,7 +412,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,59 +425,61 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>